<commit_message>
big fixes after rounding problem
</commit_message>
<xml_diff>
--- a/scr/model/par_eval/par_eval.xlsx
+++ b/scr/model/par_eval/par_eval.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlade\Documents\Github\ModelBlight\scr\model\par_eval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlade\Documents\Github\BlightModel\scr\model\par_eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3DA2E5EE-98A0-4C51-96FA-91E9B629BC9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BCF2C1-186B-4570-9416-8C2573B5F4EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-54120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="par_eval" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="30">
   <si>
     <t>met_par</t>
   </si>
@@ -115,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1056,11 +1064,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12863,7 +12871,7 @@
         <v>1</v>
       </c>
       <c r="C132" s="3" t="str">
-        <f t="shared" ref="C132:C184" si="2">_xlfn.CONCAT(A132,B132, "l")</f>
+        <f t="shared" ref="C132:C135" si="2">_xlfn.CONCAT(A132,B132, "l")</f>
         <v>ShapeSpor1l</v>
       </c>
       <c r="D132">
@@ -13126,92 +13134,89 @@
       </c>
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
-        <v>21</v>
-      </c>
-      <c r="B135">
-        <v>4</v>
+      <c r="B135" s="3">
+        <v>-3</v>
       </c>
       <c r="C135" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>ShapeSpor4l</v>
-      </c>
-      <c r="D135">
-        <v>6</v>
-      </c>
-      <c r="E135">
-        <v>12</v>
-      </c>
-      <c r="F135">
-        <v>26</v>
-      </c>
-      <c r="G135">
-        <v>1</v>
-      </c>
-      <c r="H135">
-        <v>15</v>
-      </c>
-      <c r="I135">
-        <v>6</v>
-      </c>
-      <c r="J135">
-        <v>21</v>
-      </c>
-      <c r="K135">
-        <v>26</v>
-      </c>
-      <c r="L135">
-        <v>0.6</v>
-      </c>
-      <c r="M135">
-        <v>15</v>
-      </c>
-      <c r="N135">
+        <f>_xlfn.CONCAT(A136,B135, "l")</f>
+        <v>n0Spor-3l</v>
+      </c>
+      <c r="D135" s="3">
+        <v>6</v>
+      </c>
+      <c r="E135" s="3">
+        <v>12</v>
+      </c>
+      <c r="F135" s="3">
+        <v>26</v>
+      </c>
+      <c r="G135" s="3">
+        <v>1</v>
+      </c>
+      <c r="H135" s="3">
+        <v>15</v>
+      </c>
+      <c r="I135" s="3">
+        <v>6</v>
+      </c>
+      <c r="J135" s="3">
+        <v>21</v>
+      </c>
+      <c r="K135" s="3">
+        <v>26</v>
+      </c>
+      <c r="L135" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="M135" s="3">
+        <v>15</v>
+      </c>
+      <c r="N135" s="3">
         <v>86</v>
       </c>
-      <c r="O135">
+      <c r="O135" s="3">
         <v>95</v>
       </c>
-      <c r="P135">
+      <c r="P135" s="3">
         <v>2.37</v>
       </c>
-      <c r="Q135">
+      <c r="Q135" s="3">
         <v>0.45</v>
       </c>
-      <c r="R135">
-        <v>6</v>
-      </c>
-      <c r="S135">
-        <v>20</v>
-      </c>
-      <c r="T135">
-        <v>26</v>
-      </c>
-      <c r="U135">
-        <v>1</v>
-      </c>
-      <c r="V135" s="18">
-        <v>16</v>
-      </c>
-      <c r="W135">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X135" s="1">
-        <v>6.0499999999999996E-4</v>
-      </c>
-      <c r="Y135">
+      <c r="R135" s="3">
+        <v>6</v>
+      </c>
+      <c r="S135" s="3">
+        <v>20</v>
+      </c>
+      <c r="T135" s="3">
+        <v>26</v>
+      </c>
+      <c r="U135" s="3">
+        <v>1</v>
+      </c>
+      <c r="V135" s="3">
+        <v>2</v>
+      </c>
+      <c r="W135" s="3">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X135" s="19">
+        <v>6.0500000000000003E-7</v>
+      </c>
+      <c r="Y135" s="3">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z135">
-        <v>10</v>
-      </c>
-      <c r="AA135">
-        <v>5</v>
-      </c>
-      <c r="AB135">
-        <v>5</v>
-      </c>
-      <c r="AC135">
+      <c r="Z135" s="3">
+        <v>10</v>
+      </c>
+      <c r="AA135" s="3">
+        <v>5</v>
+      </c>
+      <c r="AB135" s="3">
+        <v>5</v>
+      </c>
+      <c r="AC135" s="3">
         <v>5</v>
       </c>
     </row>
@@ -13219,89 +13224,89 @@
       <c r="A136" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B136" s="3">
-        <v>-3</v>
+      <c r="B136" s="6">
+        <v>-2</v>
       </c>
       <c r="C136" s="3" t="str">
-        <f>_xlfn.CONCAT(A136,B136, "l")</f>
-        <v>n0Spor-3l</v>
-      </c>
-      <c r="D136" s="3">
-        <v>6</v>
-      </c>
-      <c r="E136" s="3">
-        <v>12</v>
-      </c>
-      <c r="F136" s="3">
-        <v>26</v>
-      </c>
-      <c r="G136" s="3">
-        <v>1</v>
-      </c>
-      <c r="H136" s="3">
-        <v>15</v>
-      </c>
-      <c r="I136" s="3">
-        <v>6</v>
-      </c>
-      <c r="J136" s="3">
-        <v>21</v>
-      </c>
-      <c r="K136" s="3">
-        <v>26</v>
-      </c>
-      <c r="L136" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="M136" s="3">
-        <v>15</v>
-      </c>
-      <c r="N136" s="3">
+        <f>_xlfn.CONCAT(A137,B136, "l")</f>
+        <v>n0Spor-2l</v>
+      </c>
+      <c r="D136" s="6">
+        <v>6</v>
+      </c>
+      <c r="E136" s="6">
+        <v>12</v>
+      </c>
+      <c r="F136" s="6">
+        <v>26</v>
+      </c>
+      <c r="G136" s="6">
+        <v>1</v>
+      </c>
+      <c r="H136" s="6">
+        <v>15</v>
+      </c>
+      <c r="I136" s="6">
+        <v>6</v>
+      </c>
+      <c r="J136" s="6">
+        <v>21</v>
+      </c>
+      <c r="K136" s="6">
+        <v>26</v>
+      </c>
+      <c r="L136" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="M136" s="6">
+        <v>15</v>
+      </c>
+      <c r="N136" s="6">
         <v>86</v>
       </c>
-      <c r="O136" s="3">
+      <c r="O136" s="6">
         <v>95</v>
       </c>
-      <c r="P136" s="3">
+      <c r="P136" s="6">
         <v>2.37</v>
       </c>
-      <c r="Q136" s="3">
+      <c r="Q136" s="6">
         <v>0.45</v>
       </c>
-      <c r="R136" s="3">
-        <v>6</v>
-      </c>
-      <c r="S136" s="3">
-        <v>20</v>
-      </c>
-      <c r="T136" s="3">
-        <v>26</v>
-      </c>
-      <c r="U136" s="3">
-        <v>1</v>
-      </c>
-      <c r="V136" s="3">
-        <v>2</v>
-      </c>
-      <c r="W136" s="3">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X136" s="19">
-        <v>6.0500000000000003E-7</v>
-      </c>
-      <c r="Y136" s="3">
+      <c r="R136" s="6">
+        <v>6</v>
+      </c>
+      <c r="S136" s="6">
+        <v>20</v>
+      </c>
+      <c r="T136" s="6">
+        <v>26</v>
+      </c>
+      <c r="U136" s="6">
+        <v>1</v>
+      </c>
+      <c r="V136" s="6">
+        <v>2</v>
+      </c>
+      <c r="W136" s="6">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X136" s="20">
+        <v>6.0499999999999997E-6</v>
+      </c>
+      <c r="Y136" s="6">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z136" s="3">
-        <v>10</v>
-      </c>
-      <c r="AA136" s="3">
-        <v>5</v>
-      </c>
-      <c r="AB136" s="3">
-        <v>5</v>
-      </c>
-      <c r="AC136" s="3">
+      <c r="Z136" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA136" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB136" s="6">
+        <v>5</v>
+      </c>
+      <c r="AC136" s="6">
         <v>5</v>
       </c>
     </row>
@@ -13310,11 +13315,11 @@
         <v>23</v>
       </c>
       <c r="B137" s="6">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C137" s="3" t="str">
-        <f>_xlfn.CONCAT(A137,B137, "l")</f>
-        <v>n0Spor-2l</v>
+        <f>_xlfn.CONCAT(A138,B137, "l")</f>
+        <v>n0Spor-1l</v>
       </c>
       <c r="D137" s="6">
         <v>6</v>
@@ -13377,7 +13382,7 @@
         <v>97049.814199999993</v>
       </c>
       <c r="X137" s="20">
-        <v>6.0499999999999997E-6</v>
+        <v>6.05E-5</v>
       </c>
       <c r="Y137" s="6">
         <v>1.7349235380000001</v>
@@ -13400,11 +13405,11 @@
         <v>23</v>
       </c>
       <c r="B138" s="6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C138" s="3" t="str">
-        <f>_xlfn.CONCAT(A138,B138, "l")</f>
-        <v>n0Spor-1l</v>
+        <f>_xlfn.CONCAT(A139,B138, "l")</f>
+        <v>n0Spor0l</v>
       </c>
       <c r="D138" s="6">
         <v>6</v>
@@ -13467,7 +13472,7 @@
         <v>97049.814199999993</v>
       </c>
       <c r="X138" s="20">
-        <v>6.05E-5</v>
+        <v>6.0499999999999996E-4</v>
       </c>
       <c r="Y138" s="6">
         <v>1.7349235380000001</v>
@@ -13490,11 +13495,11 @@
         <v>23</v>
       </c>
       <c r="B139" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C139" s="3" t="str">
-        <f>_xlfn.CONCAT(A139,B139, "l")</f>
-        <v>n0Spor0l</v>
+        <f>_xlfn.CONCAT(A140,B139, "l")</f>
+        <v>n0Spor1l</v>
       </c>
       <c r="D139" s="6">
         <v>6</v>
@@ -13557,7 +13562,7 @@
         <v>97049.814199999993</v>
       </c>
       <c r="X139" s="20">
-        <v>6.0499999999999996E-4</v>
+        <v>6.0499999999999998E-3</v>
       </c>
       <c r="Y139" s="6">
         <v>1.7349235380000001</v>
@@ -13580,11 +13585,11 @@
         <v>23</v>
       </c>
       <c r="B140" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C140" s="3" t="str">
-        <f>_xlfn.CONCAT(A140,B140, "l")</f>
-        <v>n0Spor1l</v>
+        <f>_xlfn.CONCAT(A141,B140, "l")</f>
+        <v>n0Spor2l</v>
       </c>
       <c r="D140" s="6">
         <v>6</v>
@@ -13647,7 +13652,7 @@
         <v>97049.814199999993</v>
       </c>
       <c r="X140" s="20">
-        <v>6.0499999999999998E-3</v>
+        <v>6.0499999999999998E-2</v>
       </c>
       <c r="Y140" s="6">
         <v>1.7349235380000001</v>
@@ -13669,89 +13674,89 @@
       <c r="A141" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B141" s="6">
-        <v>2</v>
+      <c r="B141" s="9">
+        <v>3</v>
       </c>
       <c r="C141" s="3" t="str">
-        <f>_xlfn.CONCAT(A141,B141, "l")</f>
-        <v>n0Spor2l</v>
-      </c>
-      <c r="D141" s="6">
-        <v>6</v>
-      </c>
-      <c r="E141" s="6">
-        <v>12</v>
-      </c>
-      <c r="F141" s="6">
-        <v>26</v>
-      </c>
-      <c r="G141" s="6">
-        <v>1</v>
-      </c>
-      <c r="H141" s="6">
-        <v>15</v>
-      </c>
-      <c r="I141" s="6">
-        <v>6</v>
-      </c>
-      <c r="J141" s="6">
-        <v>21</v>
-      </c>
-      <c r="K141" s="6">
-        <v>26</v>
-      </c>
-      <c r="L141" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="M141" s="6">
-        <v>15</v>
-      </c>
-      <c r="N141" s="6">
+        <f>_xlfn.CONCAT(A142,B141, "l")</f>
+        <v>n0Spor3l</v>
+      </c>
+      <c r="D141" s="9">
+        <v>6</v>
+      </c>
+      <c r="E141" s="9">
+        <v>12</v>
+      </c>
+      <c r="F141" s="9">
+        <v>26</v>
+      </c>
+      <c r="G141" s="9">
+        <v>1</v>
+      </c>
+      <c r="H141" s="9">
+        <v>15</v>
+      </c>
+      <c r="I141" s="9">
+        <v>6</v>
+      </c>
+      <c r="J141" s="9">
+        <v>21</v>
+      </c>
+      <c r="K141" s="9">
+        <v>26</v>
+      </c>
+      <c r="L141" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="M141" s="9">
+        <v>15</v>
+      </c>
+      <c r="N141" s="9">
         <v>86</v>
       </c>
-      <c r="O141" s="6">
+      <c r="O141" s="9">
         <v>95</v>
       </c>
-      <c r="P141" s="6">
+      <c r="P141" s="9">
         <v>2.37</v>
       </c>
-      <c r="Q141" s="6">
+      <c r="Q141" s="9">
         <v>0.45</v>
       </c>
-      <c r="R141" s="6">
-        <v>6</v>
-      </c>
-      <c r="S141" s="6">
-        <v>20</v>
-      </c>
-      <c r="T141" s="6">
-        <v>26</v>
-      </c>
-      <c r="U141" s="6">
-        <v>1</v>
-      </c>
-      <c r="V141" s="6">
-        <v>2</v>
-      </c>
-      <c r="W141" s="6">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X141" s="20">
-        <v>6.0499999999999998E-2</v>
-      </c>
-      <c r="Y141" s="6">
+      <c r="R141" s="9">
+        <v>6</v>
+      </c>
+      <c r="S141" s="9">
+        <v>20</v>
+      </c>
+      <c r="T141" s="9">
+        <v>26</v>
+      </c>
+      <c r="U141" s="9">
+        <v>1</v>
+      </c>
+      <c r="V141" s="9">
+        <v>2</v>
+      </c>
+      <c r="W141" s="9">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X141" s="21">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="Y141" s="9">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z141" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA141" s="6">
-        <v>5</v>
-      </c>
-      <c r="AB141" s="6">
-        <v>5</v>
-      </c>
-      <c r="AC141" s="6">
+      <c r="Z141" s="9">
+        <v>10</v>
+      </c>
+      <c r="AA141" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB141" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC141" s="9">
         <v>5</v>
       </c>
     </row>
@@ -13759,89 +13764,89 @@
       <c r="A142" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B142" s="9">
-        <v>3</v>
+      <c r="B142" s="6">
+        <v>-3</v>
       </c>
       <c r="C142" s="3" t="str">
-        <f>_xlfn.CONCAT(A142,B142, "l")</f>
-        <v>n0Spor3l</v>
-      </c>
-      <c r="D142" s="9">
-        <v>6</v>
-      </c>
-      <c r="E142" s="9">
-        <v>12</v>
-      </c>
-      <c r="F142" s="9">
-        <v>26</v>
-      </c>
-      <c r="G142" s="9">
-        <v>1</v>
-      </c>
-      <c r="H142" s="9">
-        <v>15</v>
-      </c>
-      <c r="I142" s="9">
-        <v>6</v>
-      </c>
-      <c r="J142" s="9">
-        <v>21</v>
-      </c>
-      <c r="K142" s="9">
-        <v>26</v>
-      </c>
-      <c r="L142" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="M142" s="9">
-        <v>15</v>
-      </c>
-      <c r="N142" s="9">
+        <f>_xlfn.CONCAT(A143,B142, "l")</f>
+        <v>rSpor-3l</v>
+      </c>
+      <c r="D142" s="6">
+        <v>6</v>
+      </c>
+      <c r="E142" s="6">
+        <v>12</v>
+      </c>
+      <c r="F142" s="6">
+        <v>26</v>
+      </c>
+      <c r="G142" s="6">
+        <v>1</v>
+      </c>
+      <c r="H142" s="6">
+        <v>15</v>
+      </c>
+      <c r="I142" s="6">
+        <v>6</v>
+      </c>
+      <c r="J142" s="6">
+        <v>21</v>
+      </c>
+      <c r="K142" s="6">
+        <v>26</v>
+      </c>
+      <c r="L142" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="M142" s="6">
+        <v>15</v>
+      </c>
+      <c r="N142" s="6">
         <v>86</v>
       </c>
-      <c r="O142" s="9">
+      <c r="O142" s="6">
         <v>95</v>
       </c>
-      <c r="P142" s="9">
+      <c r="P142" s="6">
         <v>2.37</v>
       </c>
-      <c r="Q142" s="9">
+      <c r="Q142" s="6">
         <v>0.45</v>
       </c>
-      <c r="R142" s="9">
-        <v>6</v>
-      </c>
-      <c r="S142" s="9">
-        <v>20</v>
-      </c>
-      <c r="T142" s="9">
-        <v>26</v>
-      </c>
-      <c r="U142" s="9">
-        <v>1</v>
-      </c>
-      <c r="V142" s="9">
-        <v>2</v>
-      </c>
-      <c r="W142" s="9">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X142" s="21">
-        <v>0.60499999999999998</v>
-      </c>
-      <c r="Y142" s="9">
-        <v>1.7349235380000001</v>
-      </c>
-      <c r="Z142" s="9">
-        <v>10</v>
-      </c>
-      <c r="AA142" s="9">
-        <v>5</v>
-      </c>
-      <c r="AB142" s="9">
-        <v>5</v>
-      </c>
-      <c r="AC142" s="9">
+      <c r="R142" s="6">
+        <v>6</v>
+      </c>
+      <c r="S142" s="6">
+        <v>20</v>
+      </c>
+      <c r="T142" s="6">
+        <v>26</v>
+      </c>
+      <c r="U142" s="6">
+        <v>1</v>
+      </c>
+      <c r="V142" s="6">
+        <v>2</v>
+      </c>
+      <c r="W142" s="6">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X142" s="7">
+        <v>6.0499999999999996E-4</v>
+      </c>
+      <c r="Y142" s="16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z142" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA142" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB142" s="6">
+        <v>5</v>
+      </c>
+      <c r="AC142" s="12">
         <v>5</v>
       </c>
     </row>
@@ -13850,11 +13855,11 @@
         <v>24</v>
       </c>
       <c r="B143" s="6">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C143" s="3" t="str">
-        <f>_xlfn.CONCAT(A143,B143, "l")</f>
-        <v>rSpor-3l</v>
+        <f>_xlfn.CONCAT(A144,B143, "l")</f>
+        <v>rSpor-2l</v>
       </c>
       <c r="D143" s="6">
         <v>6</v>
@@ -13920,7 +13925,7 @@
         <v>6.0499999999999996E-4</v>
       </c>
       <c r="Y143" s="16">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="Z143" s="6">
         <v>10</v>
@@ -13940,11 +13945,11 @@
         <v>24</v>
       </c>
       <c r="B144" s="6">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C144" s="3" t="str">
-        <f>_xlfn.CONCAT(A144,B144, "l")</f>
-        <v>rSpor-2l</v>
+        <f>_xlfn.CONCAT(A145,B144, "l")</f>
+        <v>rSpor-1l</v>
       </c>
       <c r="D144" s="6">
         <v>6</v>
@@ -14010,7 +14015,7 @@
         <v>6.0499999999999996E-4</v>
       </c>
       <c r="Y144" s="16">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="Z144" s="6">
         <v>10</v>
@@ -14030,11 +14035,11 @@
         <v>24</v>
       </c>
       <c r="B145" s="6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C145" s="3" t="str">
-        <f>_xlfn.CONCAT(A145,B145, "l")</f>
-        <v>rSpor-1l</v>
+        <f>_xlfn.CONCAT(A146,B145, "l")</f>
+        <v>rSpor0l</v>
       </c>
       <c r="D145" s="6">
         <v>6</v>
@@ -14100,7 +14105,7 @@
         <v>6.0499999999999996E-4</v>
       </c>
       <c r="Y145" s="16">
-        <v>1.5</v>
+        <v>1.7349235380000001</v>
       </c>
       <c r="Z145" s="6">
         <v>10</v>
@@ -14120,11 +14125,11 @@
         <v>24</v>
       </c>
       <c r="B146" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C146" s="3" t="str">
-        <f>_xlfn.CONCAT(A146,B146, "l")</f>
-        <v>rSpor0l</v>
+        <f>_xlfn.CONCAT(A147,B146, "l")</f>
+        <v>rSpor1l</v>
       </c>
       <c r="D146" s="6">
         <v>6</v>
@@ -14190,7 +14195,7 @@
         <v>6.0499999999999996E-4</v>
       </c>
       <c r="Y146" s="16">
-        <v>1.7349235380000001</v>
+        <v>2</v>
       </c>
       <c r="Z146" s="6">
         <v>10</v>
@@ -14210,11 +14215,11 @@
         <v>24</v>
       </c>
       <c r="B147" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C147" s="3" t="str">
-        <f>_xlfn.CONCAT(A147,B147, "l")</f>
-        <v>rSpor1l</v>
+        <f>_xlfn.CONCAT(A148,B147, "l")</f>
+        <v>rSpor2l</v>
       </c>
       <c r="D147" s="6">
         <v>6</v>
@@ -14280,7 +14285,7 @@
         <v>6.0499999999999996E-4</v>
       </c>
       <c r="Y147" s="16">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Z147" s="6">
         <v>10</v>
@@ -14299,89 +14304,89 @@
       <c r="A148" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B148" s="6">
-        <v>2</v>
+      <c r="B148" s="9">
+        <v>3</v>
       </c>
       <c r="C148" s="3" t="str">
-        <f>_xlfn.CONCAT(A148,B148, "l")</f>
-        <v>rSpor2l</v>
-      </c>
-      <c r="D148" s="6">
-        <v>6</v>
-      </c>
-      <c r="E148" s="6">
-        <v>12</v>
-      </c>
-      <c r="F148" s="6">
-        <v>26</v>
-      </c>
-      <c r="G148" s="6">
-        <v>1</v>
-      </c>
-      <c r="H148" s="6">
-        <v>15</v>
-      </c>
-      <c r="I148" s="6">
-        <v>6</v>
-      </c>
-      <c r="J148" s="6">
-        <v>21</v>
-      </c>
-      <c r="K148" s="6">
-        <v>26</v>
-      </c>
-      <c r="L148" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="M148" s="6">
-        <v>15</v>
-      </c>
-      <c r="N148" s="6">
+        <f>_xlfn.CONCAT(A149,B148, "l")</f>
+        <v>rSpor3l</v>
+      </c>
+      <c r="D148" s="9">
+        <v>6</v>
+      </c>
+      <c r="E148" s="9">
+        <v>12</v>
+      </c>
+      <c r="F148" s="9">
+        <v>26</v>
+      </c>
+      <c r="G148" s="9">
+        <v>1</v>
+      </c>
+      <c r="H148" s="9">
+        <v>15</v>
+      </c>
+      <c r="I148" s="9">
+        <v>6</v>
+      </c>
+      <c r="J148" s="9">
+        <v>21</v>
+      </c>
+      <c r="K148" s="9">
+        <v>26</v>
+      </c>
+      <c r="L148" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="M148" s="9">
+        <v>15</v>
+      </c>
+      <c r="N148" s="9">
         <v>86</v>
       </c>
-      <c r="O148" s="6">
+      <c r="O148" s="9">
         <v>95</v>
       </c>
-      <c r="P148" s="6">
+      <c r="P148" s="9">
         <v>2.37</v>
       </c>
-      <c r="Q148" s="6">
+      <c r="Q148" s="9">
         <v>0.45</v>
       </c>
-      <c r="R148" s="6">
-        <v>6</v>
-      </c>
-      <c r="S148" s="6">
-        <v>20</v>
-      </c>
-      <c r="T148" s="6">
-        <v>26</v>
-      </c>
-      <c r="U148" s="6">
-        <v>1</v>
-      </c>
-      <c r="V148" s="6">
-        <v>2</v>
-      </c>
-      <c r="W148" s="6">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X148" s="7">
+      <c r="R148" s="9">
+        <v>6</v>
+      </c>
+      <c r="S148" s="9">
+        <v>20</v>
+      </c>
+      <c r="T148" s="9">
+        <v>26</v>
+      </c>
+      <c r="U148" s="9">
+        <v>1</v>
+      </c>
+      <c r="V148" s="9">
+        <v>2</v>
+      </c>
+      <c r="W148" s="9">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X148" s="10">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y148" s="16">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="Z148" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA148" s="6">
-        <v>5</v>
-      </c>
-      <c r="AB148" s="6">
-        <v>5</v>
-      </c>
-      <c r="AC148" s="12">
+      <c r="Y148" s="17">
+        <v>2.7</v>
+      </c>
+      <c r="Z148" s="9">
+        <v>10</v>
+      </c>
+      <c r="AA148" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB148" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC148" s="13">
         <v>5</v>
       </c>
     </row>
@@ -14389,89 +14394,89 @@
       <c r="A149" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B149" s="9">
-        <v>3</v>
+      <c r="B149">
+        <v>-3</v>
       </c>
       <c r="C149" s="3" t="str">
-        <f>_xlfn.CONCAT(A149,B149, "l")</f>
-        <v>rSpor3l</v>
-      </c>
-      <c r="D149" s="9">
-        <v>6</v>
-      </c>
-      <c r="E149" s="9">
-        <v>12</v>
-      </c>
-      <c r="F149" s="9">
-        <v>26</v>
-      </c>
-      <c r="G149" s="9">
-        <v>1</v>
-      </c>
-      <c r="H149" s="9">
-        <v>15</v>
-      </c>
-      <c r="I149" s="9">
-        <v>6</v>
-      </c>
-      <c r="J149" s="9">
-        <v>21</v>
-      </c>
-      <c r="K149" s="9">
-        <v>26</v>
-      </c>
-      <c r="L149" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="M149" s="9">
-        <v>15</v>
-      </c>
-      <c r="N149" s="9">
+        <f>_xlfn.CONCAT(A150,B149, "l")</f>
+        <v>spor_dur-3l</v>
+      </c>
+      <c r="D149">
+        <v>6</v>
+      </c>
+      <c r="E149">
+        <v>12</v>
+      </c>
+      <c r="F149">
+        <v>26</v>
+      </c>
+      <c r="G149">
+        <v>1</v>
+      </c>
+      <c r="H149">
+        <v>15</v>
+      </c>
+      <c r="I149">
+        <v>6</v>
+      </c>
+      <c r="J149">
+        <v>21</v>
+      </c>
+      <c r="K149">
+        <v>26</v>
+      </c>
+      <c r="L149">
+        <v>0.6</v>
+      </c>
+      <c r="M149">
+        <v>15</v>
+      </c>
+      <c r="N149">
         <v>86</v>
       </c>
-      <c r="O149" s="9">
+      <c r="O149">
         <v>95</v>
       </c>
-      <c r="P149" s="9">
+      <c r="P149">
         <v>2.37</v>
       </c>
-      <c r="Q149" s="9">
+      <c r="Q149">
         <v>0.45</v>
       </c>
-      <c r="R149" s="9">
-        <v>6</v>
-      </c>
-      <c r="S149" s="9">
-        <v>20</v>
-      </c>
-      <c r="T149" s="9">
-        <v>26</v>
-      </c>
-      <c r="U149" s="9">
-        <v>1</v>
-      </c>
-      <c r="V149" s="9">
-        <v>2</v>
-      </c>
-      <c r="W149" s="9">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X149" s="10">
+      <c r="R149">
+        <v>6</v>
+      </c>
+      <c r="S149">
+        <v>20</v>
+      </c>
+      <c r="T149">
+        <v>26</v>
+      </c>
+      <c r="U149">
+        <v>1</v>
+      </c>
+      <c r="V149">
+        <v>2</v>
+      </c>
+      <c r="W149">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X149" s="1">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y149" s="17">
-        <v>2.7</v>
-      </c>
-      <c r="Z149" s="9">
-        <v>10</v>
-      </c>
-      <c r="AA149" s="9">
-        <v>5</v>
-      </c>
-      <c r="AB149" s="9">
-        <v>5</v>
-      </c>
-      <c r="AC149" s="13">
+      <c r="Y149">
+        <v>1.7349235380000001</v>
+      </c>
+      <c r="Z149" s="18">
+        <v>4</v>
+      </c>
+      <c r="AA149">
+        <v>5</v>
+      </c>
+      <c r="AB149">
+        <v>5</v>
+      </c>
+      <c r="AC149">
         <v>5</v>
       </c>
     </row>
@@ -14480,11 +14485,11 @@
         <v>29</v>
       </c>
       <c r="B150">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C150" s="3" t="str">
-        <f>_xlfn.CONCAT(A150,B150, "l")</f>
-        <v>spor_dur-3l</v>
+        <f>_xlfn.CONCAT(A151,B150, "l")</f>
+        <v>spor_dur-2l</v>
       </c>
       <c r="D150">
         <v>6</v>
@@ -14553,7 +14558,7 @@
         <v>1.7349235380000001</v>
       </c>
       <c r="Z150" s="18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AA150">
         <v>5</v>
@@ -14570,11 +14575,11 @@
         <v>29</v>
       </c>
       <c r="B151">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C151" s="3" t="str">
-        <f>_xlfn.CONCAT(A151,B151, "l")</f>
-        <v>spor_dur-2l</v>
+        <f>_xlfn.CONCAT(A152,B151, "l")</f>
+        <v>spor_dur-1l</v>
       </c>
       <c r="D151">
         <v>6</v>
@@ -14643,7 +14648,7 @@
         <v>1.7349235380000001</v>
       </c>
       <c r="Z151" s="18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AA151">
         <v>5</v>
@@ -14660,11 +14665,11 @@
         <v>29</v>
       </c>
       <c r="B152">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C152" s="3" t="str">
-        <f>_xlfn.CONCAT(A152,B152, "l")</f>
-        <v>spor_dur-1l</v>
+        <f>_xlfn.CONCAT(A153,B152, "l")</f>
+        <v>spor_dur0l</v>
       </c>
       <c r="D152">
         <v>6</v>
@@ -14733,7 +14738,7 @@
         <v>1.7349235380000001</v>
       </c>
       <c r="Z152" s="18">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AA152">
         <v>5</v>
@@ -14750,11 +14755,11 @@
         <v>29</v>
       </c>
       <c r="B153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C153" s="3" t="str">
-        <f>_xlfn.CONCAT(A153,B153, "l")</f>
-        <v>spor_dur0l</v>
+        <f>_xlfn.CONCAT(A154,B153, "l")</f>
+        <v>spor_dur1l</v>
       </c>
       <c r="D153">
         <v>6</v>
@@ -14823,7 +14828,7 @@
         <v>1.7349235380000001</v>
       </c>
       <c r="Z153" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA153">
         <v>5</v>
@@ -14840,11 +14845,11 @@
         <v>29</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C154" s="3" t="str">
-        <f>_xlfn.CONCAT(A154,B154, "l")</f>
-        <v>spor_dur1l</v>
+        <f>_xlfn.CONCAT(A155,B154, "l")</f>
+        <v>spor_dur2l</v>
       </c>
       <c r="D154">
         <v>6</v>
@@ -14913,7 +14918,7 @@
         <v>1.7349235380000001</v>
       </c>
       <c r="Z154" s="18">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AA154">
         <v>5</v>
@@ -14930,11 +14935,11 @@
         <v>29</v>
       </c>
       <c r="B155">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C155" s="3" t="str">
-        <f>_xlfn.CONCAT(A155,B155, "l")</f>
-        <v>spor_dur2l</v>
+        <f>_xlfn.CONCAT(A156,B155, "l")</f>
+        <v>spor_dur3l</v>
       </c>
       <c r="D155">
         <v>6</v>
@@ -15003,7 +15008,7 @@
         <v>1.7349235380000001</v>
       </c>
       <c r="Z155" s="18">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AA155">
         <v>5</v>
@@ -15019,89 +15024,89 @@
       <c r="A156" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B156">
-        <v>3</v>
+      <c r="B156" s="3">
+        <v>-3</v>
       </c>
       <c r="C156" s="3" t="str">
-        <f>_xlfn.CONCAT(A156,B156, "l")</f>
-        <v>spor_dur3l</v>
-      </c>
-      <c r="D156">
-        <v>6</v>
-      </c>
-      <c r="E156">
-        <v>12</v>
-      </c>
-      <c r="F156">
-        <v>26</v>
-      </c>
-      <c r="G156">
-        <v>1</v>
-      </c>
-      <c r="H156">
-        <v>15</v>
-      </c>
-      <c r="I156">
-        <v>6</v>
-      </c>
-      <c r="J156">
-        <v>21</v>
-      </c>
-      <c r="K156">
-        <v>26</v>
-      </c>
-      <c r="L156">
-        <v>0.6</v>
-      </c>
-      <c r="M156">
-        <v>15</v>
-      </c>
-      <c r="N156">
+        <f>_xlfn.CONCAT(A157,B156, "l")</f>
+        <v>hr_before_spor-3l</v>
+      </c>
+      <c r="D156" s="3">
+        <v>6</v>
+      </c>
+      <c r="E156" s="3">
+        <v>12</v>
+      </c>
+      <c r="F156" s="3">
+        <v>26</v>
+      </c>
+      <c r="G156" s="3">
+        <v>1</v>
+      </c>
+      <c r="H156" s="3">
+        <v>15</v>
+      </c>
+      <c r="I156" s="3">
+        <v>6</v>
+      </c>
+      <c r="J156" s="3">
+        <v>21</v>
+      </c>
+      <c r="K156" s="3">
+        <v>26</v>
+      </c>
+      <c r="L156" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="M156" s="3">
+        <v>15</v>
+      </c>
+      <c r="N156" s="3">
         <v>86</v>
       </c>
-      <c r="O156">
+      <c r="O156" s="3">
         <v>95</v>
       </c>
-      <c r="P156">
+      <c r="P156" s="3">
         <v>2.37</v>
       </c>
-      <c r="Q156">
+      <c r="Q156" s="3">
         <v>0.45</v>
       </c>
-      <c r="R156">
-        <v>6</v>
-      </c>
-      <c r="S156">
-        <v>20</v>
-      </c>
-      <c r="T156">
-        <v>26</v>
-      </c>
-      <c r="U156">
-        <v>1</v>
-      </c>
-      <c r="V156">
-        <v>2</v>
-      </c>
-      <c r="W156">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X156" s="1">
+      <c r="R156" s="3">
+        <v>6</v>
+      </c>
+      <c r="S156" s="3">
+        <v>20</v>
+      </c>
+      <c r="T156" s="3">
+        <v>26</v>
+      </c>
+      <c r="U156" s="3">
+        <v>1</v>
+      </c>
+      <c r="V156" s="3">
+        <v>2</v>
+      </c>
+      <c r="W156" s="3">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X156" s="4">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y156">
+      <c r="Y156" s="3">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z156" s="18">
-        <v>16</v>
-      </c>
-      <c r="AA156">
-        <v>5</v>
-      </c>
-      <c r="AB156">
-        <v>5</v>
-      </c>
-      <c r="AC156">
+      <c r="Z156" s="3">
+        <v>10</v>
+      </c>
+      <c r="AA156" s="15">
+        <v>2</v>
+      </c>
+      <c r="AB156" s="3">
+        <v>5</v>
+      </c>
+      <c r="AC156" s="11">
         <v>5</v>
       </c>
     </row>
@@ -15109,89 +15114,89 @@
       <c r="A157" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B157" s="3">
-        <v>-3</v>
+      <c r="B157" s="6">
+        <v>-2</v>
       </c>
       <c r="C157" s="3" t="str">
-        <f>_xlfn.CONCAT(A157,B157, "l")</f>
-        <v>hr_before_spor-3l</v>
-      </c>
-      <c r="D157" s="3">
-        <v>6</v>
-      </c>
-      <c r="E157" s="3">
-        <v>12</v>
-      </c>
-      <c r="F157" s="3">
-        <v>26</v>
-      </c>
-      <c r="G157" s="3">
-        <v>1</v>
-      </c>
-      <c r="H157" s="3">
-        <v>15</v>
-      </c>
-      <c r="I157" s="3">
-        <v>6</v>
-      </c>
-      <c r="J157" s="3">
-        <v>21</v>
-      </c>
-      <c r="K157" s="3">
-        <v>26</v>
-      </c>
-      <c r="L157" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="M157" s="3">
-        <v>15</v>
-      </c>
-      <c r="N157" s="3">
+        <f>_xlfn.CONCAT(A158,B157, "l")</f>
+        <v>hr_before_spor-2l</v>
+      </c>
+      <c r="D157" s="6">
+        <v>6</v>
+      </c>
+      <c r="E157" s="6">
+        <v>12</v>
+      </c>
+      <c r="F157" s="6">
+        <v>26</v>
+      </c>
+      <c r="G157" s="6">
+        <v>1</v>
+      </c>
+      <c r="H157" s="6">
+        <v>15</v>
+      </c>
+      <c r="I157" s="6">
+        <v>6</v>
+      </c>
+      <c r="J157" s="6">
+        <v>21</v>
+      </c>
+      <c r="K157" s="6">
+        <v>26</v>
+      </c>
+      <c r="L157" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="M157" s="6">
+        <v>15</v>
+      </c>
+      <c r="N157" s="6">
         <v>86</v>
       </c>
-      <c r="O157" s="3">
+      <c r="O157" s="6">
         <v>95</v>
       </c>
-      <c r="P157" s="3">
+      <c r="P157" s="6">
         <v>2.37</v>
       </c>
-      <c r="Q157" s="3">
+      <c r="Q157" s="6">
         <v>0.45</v>
       </c>
-      <c r="R157" s="3">
-        <v>6</v>
-      </c>
-      <c r="S157" s="3">
-        <v>20</v>
-      </c>
-      <c r="T157" s="3">
-        <v>26</v>
-      </c>
-      <c r="U157" s="3">
-        <v>1</v>
-      </c>
-      <c r="V157" s="3">
-        <v>2</v>
-      </c>
-      <c r="W157" s="3">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X157" s="4">
+      <c r="R157" s="6">
+        <v>6</v>
+      </c>
+      <c r="S157" s="6">
+        <v>20</v>
+      </c>
+      <c r="T157" s="6">
+        <v>26</v>
+      </c>
+      <c r="U157" s="6">
+        <v>1</v>
+      </c>
+      <c r="V157" s="6">
+        <v>2</v>
+      </c>
+      <c r="W157" s="6">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X157" s="7">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y157" s="3">
+      <c r="Y157" s="6">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z157" s="3">
-        <v>10</v>
-      </c>
-      <c r="AA157" s="15">
-        <v>2</v>
-      </c>
-      <c r="AB157" s="3">
-        <v>5</v>
-      </c>
-      <c r="AC157" s="11">
+      <c r="Z157" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA157" s="16">
+        <v>3</v>
+      </c>
+      <c r="AB157" s="6">
+        <v>5</v>
+      </c>
+      <c r="AC157" s="12">
         <v>5</v>
       </c>
     </row>
@@ -15200,11 +15205,11 @@
         <v>25</v>
       </c>
       <c r="B158" s="6">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C158" s="3" t="str">
-        <f>_xlfn.CONCAT(A158,B158, "l")</f>
-        <v>hr_before_spor-2l</v>
+        <f>_xlfn.CONCAT(A159,B158, "l")</f>
+        <v>hr_before_spor-1l</v>
       </c>
       <c r="D158" s="6">
         <v>6</v>
@@ -15276,7 +15281,7 @@
         <v>10</v>
       </c>
       <c r="AA158" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB158" s="6">
         <v>5</v>
@@ -15290,11 +15295,11 @@
         <v>25</v>
       </c>
       <c r="B159" s="6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C159" s="3" t="str">
-        <f>_xlfn.CONCAT(A159,B159, "l")</f>
-        <v>hr_before_spor-1l</v>
+        <f>_xlfn.CONCAT(A160,B159, "l")</f>
+        <v>hr_before_spor0l</v>
       </c>
       <c r="D159" s="6">
         <v>6</v>
@@ -15366,7 +15371,7 @@
         <v>10</v>
       </c>
       <c r="AA159" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB159" s="6">
         <v>5</v>
@@ -15380,11 +15385,11 @@
         <v>25</v>
       </c>
       <c r="B160" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C160" s="3" t="str">
-        <f>_xlfn.CONCAT(A160,B160, "l")</f>
-        <v>hr_before_spor0l</v>
+        <f>_xlfn.CONCAT(A161,B160, "l")</f>
+        <v>hr_before_spor1l</v>
       </c>
       <c r="D160" s="6">
         <v>6</v>
@@ -15456,7 +15461,7 @@
         <v>10</v>
       </c>
       <c r="AA160" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB160" s="6">
         <v>5</v>
@@ -15470,11 +15475,11 @@
         <v>25</v>
       </c>
       <c r="B161" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C161" s="3" t="str">
-        <f>_xlfn.CONCAT(A161,B161, "l")</f>
-        <v>hr_before_spor1l</v>
+        <f>_xlfn.CONCAT(A162,B161, "l")</f>
+        <v>hr_before_spor2l</v>
       </c>
       <c r="D161" s="6">
         <v>6</v>
@@ -15546,7 +15551,7 @@
         <v>10</v>
       </c>
       <c r="AA161" s="16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB161" s="6">
         <v>5</v>
@@ -15559,89 +15564,89 @@
       <c r="A162" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B162" s="6">
-        <v>2</v>
+      <c r="B162" s="9">
+        <v>3</v>
       </c>
       <c r="C162" s="3" t="str">
-        <f>_xlfn.CONCAT(A162,B162, "l")</f>
-        <v>hr_before_spor2l</v>
-      </c>
-      <c r="D162" s="6">
-        <v>6</v>
-      </c>
-      <c r="E162" s="6">
-        <v>12</v>
-      </c>
-      <c r="F162" s="6">
-        <v>26</v>
-      </c>
-      <c r="G162" s="6">
-        <v>1</v>
-      </c>
-      <c r="H162" s="6">
-        <v>15</v>
-      </c>
-      <c r="I162" s="6">
-        <v>6</v>
-      </c>
-      <c r="J162" s="6">
-        <v>21</v>
-      </c>
-      <c r="K162" s="6">
-        <v>26</v>
-      </c>
-      <c r="L162" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="M162" s="6">
-        <v>15</v>
-      </c>
-      <c r="N162" s="6">
+        <f>_xlfn.CONCAT(A163,B162, "l")</f>
+        <v>hr_before_spor3l</v>
+      </c>
+      <c r="D162" s="9">
+        <v>6</v>
+      </c>
+      <c r="E162" s="9">
+        <v>12</v>
+      </c>
+      <c r="F162" s="9">
+        <v>26</v>
+      </c>
+      <c r="G162" s="9">
+        <v>1</v>
+      </c>
+      <c r="H162" s="9">
+        <v>15</v>
+      </c>
+      <c r="I162" s="9">
+        <v>6</v>
+      </c>
+      <c r="J162" s="9">
+        <v>21</v>
+      </c>
+      <c r="K162" s="9">
+        <v>26</v>
+      </c>
+      <c r="L162" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="M162" s="9">
+        <v>15</v>
+      </c>
+      <c r="N162" s="9">
         <v>86</v>
       </c>
-      <c r="O162" s="6">
+      <c r="O162" s="9">
         <v>95</v>
       </c>
-      <c r="P162" s="6">
+      <c r="P162" s="9">
         <v>2.37</v>
       </c>
-      <c r="Q162" s="6">
+      <c r="Q162" s="9">
         <v>0.45</v>
       </c>
-      <c r="R162" s="6">
-        <v>6</v>
-      </c>
-      <c r="S162" s="6">
-        <v>20</v>
-      </c>
-      <c r="T162" s="6">
-        <v>26</v>
-      </c>
-      <c r="U162" s="6">
-        <v>1</v>
-      </c>
-      <c r="V162" s="6">
-        <v>2</v>
-      </c>
-      <c r="W162" s="6">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X162" s="7">
+      <c r="R162" s="9">
+        <v>6</v>
+      </c>
+      <c r="S162" s="9">
+        <v>20</v>
+      </c>
+      <c r="T162" s="9">
+        <v>26</v>
+      </c>
+      <c r="U162" s="9">
+        <v>1</v>
+      </c>
+      <c r="V162" s="9">
+        <v>2</v>
+      </c>
+      <c r="W162" s="9">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X162" s="10">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y162" s="6">
+      <c r="Y162" s="9">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z162" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA162" s="16">
-        <v>7</v>
-      </c>
-      <c r="AB162" s="6">
-        <v>5</v>
-      </c>
-      <c r="AC162" s="12">
+      <c r="Z162" s="9">
+        <v>10</v>
+      </c>
+      <c r="AA162" s="17">
+        <v>8</v>
+      </c>
+      <c r="AB162" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC162" s="13">
         <v>5</v>
       </c>
     </row>
@@ -15649,89 +15654,89 @@
       <c r="A163" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B163" s="9">
-        <v>3</v>
+      <c r="B163">
+        <v>-3</v>
       </c>
       <c r="C163" s="3" t="str">
-        <f>_xlfn.CONCAT(A163,B163, "l")</f>
-        <v>hr_before_spor3l</v>
-      </c>
-      <c r="D163" s="9">
-        <v>6</v>
-      </c>
-      <c r="E163" s="9">
-        <v>12</v>
-      </c>
-      <c r="F163" s="9">
-        <v>26</v>
-      </c>
-      <c r="G163" s="9">
-        <v>1</v>
-      </c>
-      <c r="H163" s="9">
-        <v>15</v>
-      </c>
-      <c r="I163" s="9">
-        <v>6</v>
-      </c>
-      <c r="J163" s="9">
-        <v>21</v>
-      </c>
-      <c r="K163" s="9">
-        <v>26</v>
-      </c>
-      <c r="L163" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="M163" s="9">
-        <v>15</v>
-      </c>
-      <c r="N163" s="9">
+        <f>_xlfn.CONCAT(A164,B163, "l")</f>
+        <v>hr_after_spor-3l</v>
+      </c>
+      <c r="D163">
+        <v>6</v>
+      </c>
+      <c r="E163">
+        <v>12</v>
+      </c>
+      <c r="F163">
+        <v>26</v>
+      </c>
+      <c r="G163">
+        <v>1</v>
+      </c>
+      <c r="H163">
+        <v>15</v>
+      </c>
+      <c r="I163">
+        <v>6</v>
+      </c>
+      <c r="J163">
+        <v>21</v>
+      </c>
+      <c r="K163">
+        <v>26</v>
+      </c>
+      <c r="L163">
+        <v>0.6</v>
+      </c>
+      <c r="M163">
+        <v>15</v>
+      </c>
+      <c r="N163">
         <v>86</v>
       </c>
-      <c r="O163" s="9">
+      <c r="O163">
         <v>95</v>
       </c>
-      <c r="P163" s="9">
+      <c r="P163">
         <v>2.37</v>
       </c>
-      <c r="Q163" s="9">
+      <c r="Q163">
         <v>0.45</v>
       </c>
-      <c r="R163" s="9">
-        <v>6</v>
-      </c>
-      <c r="S163" s="9">
-        <v>20</v>
-      </c>
-      <c r="T163" s="9">
-        <v>26</v>
-      </c>
-      <c r="U163" s="9">
-        <v>1</v>
-      </c>
-      <c r="V163" s="9">
-        <v>2</v>
-      </c>
-      <c r="W163" s="9">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X163" s="10">
+      <c r="R163">
+        <v>6</v>
+      </c>
+      <c r="S163">
+        <v>20</v>
+      </c>
+      <c r="T163">
+        <v>26</v>
+      </c>
+      <c r="U163">
+        <v>1</v>
+      </c>
+      <c r="V163">
+        <v>2</v>
+      </c>
+      <c r="W163">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X163" s="1">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y163" s="9">
+      <c r="Y163">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z163" s="9">
-        <v>10</v>
-      </c>
-      <c r="AA163" s="17">
-        <v>8</v>
-      </c>
-      <c r="AB163" s="9">
-        <v>5</v>
-      </c>
-      <c r="AC163" s="13">
+      <c r="Z163">
+        <v>10</v>
+      </c>
+      <c r="AA163">
+        <v>5</v>
+      </c>
+      <c r="AB163" s="18">
+        <v>2</v>
+      </c>
+      <c r="AC163">
         <v>5</v>
       </c>
     </row>
@@ -15740,11 +15745,11 @@
         <v>26</v>
       </c>
       <c r="B164">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C164" s="3" t="str">
-        <f>_xlfn.CONCAT(A164,B164, "l")</f>
-        <v>hr_after_spor-3l</v>
+        <f>_xlfn.CONCAT(A165,B164, "l")</f>
+        <v>hr_after_spor-2l</v>
       </c>
       <c r="D164">
         <v>6</v>
@@ -15819,7 +15824,7 @@
         <v>5</v>
       </c>
       <c r="AB164" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC164">
         <v>5</v>
@@ -15830,11 +15835,11 @@
         <v>26</v>
       </c>
       <c r="B165">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C165" s="3" t="str">
-        <f>_xlfn.CONCAT(A165,B165, "l")</f>
-        <v>hr_after_spor-2l</v>
+        <f>_xlfn.CONCAT(A166,B165, "l")</f>
+        <v>hr_after_spor-1l</v>
       </c>
       <c r="D165">
         <v>6</v>
@@ -15909,7 +15914,7 @@
         <v>5</v>
       </c>
       <c r="AB165" s="18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC165">
         <v>5</v>
@@ -15920,11 +15925,11 @@
         <v>26</v>
       </c>
       <c r="B166">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C166" s="3" t="str">
-        <f>_xlfn.CONCAT(A166,B166, "l")</f>
-        <v>hr_after_spor-1l</v>
+        <f>_xlfn.CONCAT(A167,B166, "l")</f>
+        <v>hr_after_spor0l</v>
       </c>
       <c r="D166">
         <v>6</v>
@@ -15999,7 +16004,7 @@
         <v>5</v>
       </c>
       <c r="AB166" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC166">
         <v>5</v>
@@ -16010,11 +16015,11 @@
         <v>26</v>
       </c>
       <c r="B167">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C167" s="3" t="str">
-        <f>_xlfn.CONCAT(A167,B167, "l")</f>
-        <v>hr_after_spor0l</v>
+        <f>_xlfn.CONCAT(A168,B167, "l")</f>
+        <v>hr_after_spor1l</v>
       </c>
       <c r="D167">
         <v>6</v>
@@ -16089,7 +16094,7 @@
         <v>5</v>
       </c>
       <c r="AB167" s="18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC167">
         <v>5</v>
@@ -16100,11 +16105,11 @@
         <v>26</v>
       </c>
       <c r="B168">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C168" s="3" t="str">
-        <f>_xlfn.CONCAT(A168,B168, "l")</f>
-        <v>hr_after_spor1l</v>
+        <f>_xlfn.CONCAT(A169,B168, "l")</f>
+        <v>hr_after_spor2l</v>
       </c>
       <c r="D168">
         <v>6</v>
@@ -16179,7 +16184,7 @@
         <v>5</v>
       </c>
       <c r="AB168" s="18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC168">
         <v>5</v>
@@ -16190,11 +16195,11 @@
         <v>26</v>
       </c>
       <c r="B169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C169" s="3" t="str">
-        <f>_xlfn.CONCAT(A169,B169, "l")</f>
-        <v>hr_after_spor2l</v>
+        <f>_xlfn.CONCAT(A170,B169, "l")</f>
+        <v>hr_after_spor3l</v>
       </c>
       <c r="D169">
         <v>6</v>
@@ -16269,7 +16274,7 @@
         <v>5</v>
       </c>
       <c r="AB169" s="18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC169">
         <v>5</v>
@@ -16279,180 +16284,180 @@
       <c r="A170" t="s">
         <v>26</v>
       </c>
-      <c r="B170">
-        <v>3</v>
+      <c r="B170" s="3">
+        <v>-3</v>
       </c>
       <c r="C170" s="3" t="str">
-        <f>_xlfn.CONCAT(A170,B170, "l")</f>
-        <v>hr_after_spor3l</v>
-      </c>
-      <c r="D170">
-        <v>6</v>
-      </c>
-      <c r="E170">
-        <v>12</v>
-      </c>
-      <c r="F170">
-        <v>26</v>
-      </c>
-      <c r="G170">
-        <v>1</v>
-      </c>
-      <c r="H170">
-        <v>15</v>
-      </c>
-      <c r="I170">
-        <v>6</v>
-      </c>
-      <c r="J170">
-        <v>21</v>
-      </c>
-      <c r="K170">
-        <v>26</v>
-      </c>
-      <c r="L170">
-        <v>0.6</v>
-      </c>
-      <c r="M170">
-        <v>15</v>
-      </c>
-      <c r="N170">
+        <f>_xlfn.CONCAT(A171,B170, "l")</f>
+        <v>hr_after_inf-3l</v>
+      </c>
+      <c r="D170" s="3">
+        <v>6</v>
+      </c>
+      <c r="E170" s="3">
+        <v>12</v>
+      </c>
+      <c r="F170" s="3">
+        <v>26</v>
+      </c>
+      <c r="G170" s="3">
+        <v>1</v>
+      </c>
+      <c r="H170" s="3">
+        <v>15</v>
+      </c>
+      <c r="I170" s="3">
+        <v>6</v>
+      </c>
+      <c r="J170" s="3">
+        <v>21</v>
+      </c>
+      <c r="K170" s="3">
+        <v>26</v>
+      </c>
+      <c r="L170" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="M170" s="3">
+        <v>15</v>
+      </c>
+      <c r="N170" s="3">
         <v>86</v>
       </c>
-      <c r="O170">
+      <c r="O170" s="3">
         <v>95</v>
       </c>
-      <c r="P170">
+      <c r="P170" s="3">
         <v>2.37</v>
       </c>
-      <c r="Q170">
+      <c r="Q170" s="3">
         <v>0.45</v>
       </c>
-      <c r="R170">
-        <v>6</v>
-      </c>
-      <c r="S170">
-        <v>20</v>
-      </c>
-      <c r="T170">
-        <v>26</v>
-      </c>
-      <c r="U170">
-        <v>1</v>
-      </c>
-      <c r="V170">
-        <v>2</v>
-      </c>
-      <c r="W170">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X170" s="1">
+      <c r="R170" s="3">
+        <v>6</v>
+      </c>
+      <c r="S170" s="3">
+        <v>20</v>
+      </c>
+      <c r="T170" s="3">
+        <v>26</v>
+      </c>
+      <c r="U170" s="3">
+        <v>1</v>
+      </c>
+      <c r="V170" s="3">
+        <v>2</v>
+      </c>
+      <c r="W170" s="3">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X170" s="4">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y170">
+      <c r="Y170" s="3">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z170">
-        <v>10</v>
-      </c>
-      <c r="AA170">
-        <v>5</v>
-      </c>
-      <c r="AB170" s="18">
-        <v>8</v>
-      </c>
-      <c r="AC170">
-        <v>5</v>
+      <c r="Z170" s="3">
+        <v>10</v>
+      </c>
+      <c r="AA170" s="3">
+        <v>5</v>
+      </c>
+      <c r="AB170" s="3">
+        <v>5</v>
+      </c>
+      <c r="AC170" s="15">
+        <v>2</v>
       </c>
     </row>
     <row r="171" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B171" s="3">
-        <v>-3</v>
+      <c r="B171" s="6">
+        <v>-2</v>
       </c>
       <c r="C171" s="3" t="str">
-        <f>_xlfn.CONCAT(A171,B171, "l")</f>
-        <v>hr_after_inf-3l</v>
-      </c>
-      <c r="D171" s="3">
-        <v>6</v>
-      </c>
-      <c r="E171" s="3">
-        <v>12</v>
-      </c>
-      <c r="F171" s="3">
-        <v>26</v>
-      </c>
-      <c r="G171" s="3">
-        <v>1</v>
-      </c>
-      <c r="H171" s="3">
-        <v>15</v>
-      </c>
-      <c r="I171" s="3">
-        <v>6</v>
-      </c>
-      <c r="J171" s="3">
-        <v>21</v>
-      </c>
-      <c r="K171" s="3">
-        <v>26</v>
-      </c>
-      <c r="L171" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="M171" s="3">
-        <v>15</v>
-      </c>
-      <c r="N171" s="3">
+        <f>_xlfn.CONCAT(A172,B171, "l")</f>
+        <v>hr_after_inf-2l</v>
+      </c>
+      <c r="D171" s="6">
+        <v>6</v>
+      </c>
+      <c r="E171" s="6">
+        <v>12</v>
+      </c>
+      <c r="F171" s="6">
+        <v>26</v>
+      </c>
+      <c r="G171" s="6">
+        <v>1</v>
+      </c>
+      <c r="H171" s="6">
+        <v>15</v>
+      </c>
+      <c r="I171" s="6">
+        <v>6</v>
+      </c>
+      <c r="J171" s="6">
+        <v>21</v>
+      </c>
+      <c r="K171" s="6">
+        <v>26</v>
+      </c>
+      <c r="L171" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="M171" s="6">
+        <v>15</v>
+      </c>
+      <c r="N171" s="6">
         <v>86</v>
       </c>
-      <c r="O171" s="3">
+      <c r="O171" s="6">
         <v>95</v>
       </c>
-      <c r="P171" s="3">
+      <c r="P171" s="6">
         <v>2.37</v>
       </c>
-      <c r="Q171" s="3">
+      <c r="Q171" s="6">
         <v>0.45</v>
       </c>
-      <c r="R171" s="3">
-        <v>6</v>
-      </c>
-      <c r="S171" s="3">
-        <v>20</v>
-      </c>
-      <c r="T171" s="3">
-        <v>26</v>
-      </c>
-      <c r="U171" s="3">
-        <v>1</v>
-      </c>
-      <c r="V171" s="3">
-        <v>2</v>
-      </c>
-      <c r="W171" s="3">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X171" s="4">
+      <c r="R171" s="6">
+        <v>6</v>
+      </c>
+      <c r="S171" s="6">
+        <v>20</v>
+      </c>
+      <c r="T171" s="6">
+        <v>26</v>
+      </c>
+      <c r="U171" s="6">
+        <v>1</v>
+      </c>
+      <c r="V171" s="6">
+        <v>2</v>
+      </c>
+      <c r="W171" s="6">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X171" s="7">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y171" s="3">
+      <c r="Y171" s="6">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z171" s="3">
-        <v>10</v>
-      </c>
-      <c r="AA171" s="3">
-        <v>5</v>
-      </c>
-      <c r="AB171" s="3">
-        <v>5</v>
-      </c>
-      <c r="AC171" s="15">
-        <v>2</v>
+      <c r="Z171" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA171" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB171" s="6">
+        <v>5</v>
+      </c>
+      <c r="AC171" s="16">
+        <v>3</v>
       </c>
     </row>
     <row r="172" spans="1:29" x14ac:dyDescent="0.35">
@@ -16460,11 +16465,11 @@
         <v>27</v>
       </c>
       <c r="B172" s="6">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C172" s="3" t="str">
-        <f>_xlfn.CONCAT(A172,B172, "l")</f>
-        <v>hr_after_inf-2l</v>
+        <f>_xlfn.CONCAT(A173,B172, "l")</f>
+        <v>hr_after_inf-1l</v>
       </c>
       <c r="D172" s="6">
         <v>6</v>
@@ -16542,7 +16547,7 @@
         <v>5</v>
       </c>
       <c r="AC172" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:29" x14ac:dyDescent="0.35">
@@ -16550,11 +16555,11 @@
         <v>27</v>
       </c>
       <c r="B173" s="6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C173" s="3" t="str">
-        <f>_xlfn.CONCAT(A173,B173, "l")</f>
-        <v>hr_after_inf-1l</v>
+        <f>_xlfn.CONCAT(A174,B173, "l")</f>
+        <v>hr_after_inf0l</v>
       </c>
       <c r="D173" s="6">
         <v>6</v>
@@ -16632,7 +16637,7 @@
         <v>5</v>
       </c>
       <c r="AC173" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" spans="1:29" x14ac:dyDescent="0.35">
@@ -16640,11 +16645,11 @@
         <v>27</v>
       </c>
       <c r="B174" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C174" s="3" t="str">
-        <f>_xlfn.CONCAT(A174,B174, "l")</f>
-        <v>hr_after_inf0l</v>
+        <f>_xlfn.CONCAT(A175,B174, "l")</f>
+        <v>hr_after_inf1l</v>
       </c>
       <c r="D174" s="6">
         <v>6</v>
@@ -16722,7 +16727,7 @@
         <v>5</v>
       </c>
       <c r="AC174" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="175" spans="1:29" x14ac:dyDescent="0.35">
@@ -16730,11 +16735,11 @@
         <v>27</v>
       </c>
       <c r="B175" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C175" s="3" t="str">
-        <f>_xlfn.CONCAT(A175,B175, "l")</f>
-        <v>hr_after_inf1l</v>
+        <f>_xlfn.CONCAT(A176,B175, "l")</f>
+        <v>hr_after_inf2l</v>
       </c>
       <c r="D175" s="6">
         <v>6</v>
@@ -16812,196 +16817,111 @@
         <v>5</v>
       </c>
       <c r="AC175" s="16">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="176" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B176" s="6">
-        <v>2</v>
+      <c r="B176" s="9">
+        <v>3</v>
       </c>
       <c r="C176" s="3" t="str">
-        <f>_xlfn.CONCAT(A176,B176, "l")</f>
-        <v>hr_after_inf2l</v>
-      </c>
-      <c r="D176" s="6">
-        <v>6</v>
-      </c>
-      <c r="E176" s="6">
-        <v>12</v>
-      </c>
-      <c r="F176" s="6">
-        <v>26</v>
-      </c>
-      <c r="G176" s="6">
-        <v>1</v>
-      </c>
-      <c r="H176" s="6">
-        <v>15</v>
-      </c>
-      <c r="I176" s="6">
-        <v>6</v>
-      </c>
-      <c r="J176" s="6">
-        <v>21</v>
-      </c>
-      <c r="K176" s="6">
-        <v>26</v>
-      </c>
-      <c r="L176" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="M176" s="6">
-        <v>15</v>
-      </c>
-      <c r="N176" s="6">
+        <f>_xlfn.CONCAT(A177,B176, "l")</f>
+        <v>hr_after_inf3l</v>
+      </c>
+      <c r="D176" s="9">
+        <v>6</v>
+      </c>
+      <c r="E176" s="9">
+        <v>12</v>
+      </c>
+      <c r="F176" s="9">
+        <v>26</v>
+      </c>
+      <c r="G176" s="9">
+        <v>1</v>
+      </c>
+      <c r="H176" s="9">
+        <v>15</v>
+      </c>
+      <c r="I176" s="9">
+        <v>6</v>
+      </c>
+      <c r="J176" s="9">
+        <v>21</v>
+      </c>
+      <c r="K176" s="9">
+        <v>26</v>
+      </c>
+      <c r="L176" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="M176" s="9">
+        <v>15</v>
+      </c>
+      <c r="N176" s="9">
         <v>86</v>
       </c>
-      <c r="O176" s="6">
+      <c r="O176" s="9">
         <v>95</v>
       </c>
-      <c r="P176" s="6">
+      <c r="P176" s="9">
         <v>2.37</v>
       </c>
-      <c r="Q176" s="6">
+      <c r="Q176" s="9">
         <v>0.45</v>
       </c>
-      <c r="R176" s="6">
-        <v>6</v>
-      </c>
-      <c r="S176" s="6">
-        <v>20</v>
-      </c>
-      <c r="T176" s="6">
-        <v>26</v>
-      </c>
-      <c r="U176" s="6">
-        <v>1</v>
-      </c>
-      <c r="V176" s="6">
-        <v>2</v>
-      </c>
-      <c r="W176" s="6">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X176" s="7">
+      <c r="R176" s="9">
+        <v>6</v>
+      </c>
+      <c r="S176" s="9">
+        <v>20</v>
+      </c>
+      <c r="T176" s="9">
+        <v>26</v>
+      </c>
+      <c r="U176" s="9">
+        <v>1</v>
+      </c>
+      <c r="V176" s="9">
+        <v>2</v>
+      </c>
+      <c r="W176" s="9">
+        <v>97049.814199999993</v>
+      </c>
+      <c r="X176" s="10">
         <v>6.0499999999999996E-4</v>
       </c>
-      <c r="Y176" s="6">
+      <c r="Y176" s="9">
         <v>1.7349235380000001</v>
       </c>
-      <c r="Z176" s="6">
-        <v>10</v>
-      </c>
-      <c r="AA176" s="6">
-        <v>5</v>
-      </c>
-      <c r="AB176" s="6">
-        <v>5</v>
-      </c>
-      <c r="AC176" s="16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="Z176" s="9">
+        <v>10</v>
+      </c>
+      <c r="AA176" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB176" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC176" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B177" s="9">
-        <v>3</v>
-      </c>
-      <c r="C177" s="3" t="str">
-        <f>_xlfn.CONCAT(A177,B177, "l")</f>
-        <v>hr_after_inf3l</v>
-      </c>
-      <c r="D177" s="9">
-        <v>6</v>
-      </c>
-      <c r="E177" s="9">
-        <v>12</v>
-      </c>
-      <c r="F177" s="9">
-        <v>26</v>
-      </c>
-      <c r="G177" s="9">
-        <v>1</v>
-      </c>
-      <c r="H177" s="9">
-        <v>15</v>
-      </c>
-      <c r="I177" s="9">
-        <v>6</v>
-      </c>
-      <c r="J177" s="9">
-        <v>21</v>
-      </c>
-      <c r="K177" s="9">
-        <v>26</v>
-      </c>
-      <c r="L177" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="M177" s="9">
-        <v>15</v>
-      </c>
-      <c r="N177" s="9">
-        <v>86</v>
-      </c>
-      <c r="O177" s="9">
-        <v>95</v>
-      </c>
-      <c r="P177" s="9">
-        <v>2.37</v>
-      </c>
-      <c r="Q177" s="9">
-        <v>0.45</v>
-      </c>
-      <c r="R177" s="9">
-        <v>6</v>
-      </c>
-      <c r="S177" s="9">
-        <v>20</v>
-      </c>
-      <c r="T177" s="9">
-        <v>26</v>
-      </c>
-      <c r="U177" s="9">
-        <v>1</v>
-      </c>
-      <c r="V177" s="9">
-        <v>2</v>
-      </c>
-      <c r="W177" s="9">
-        <v>97049.814199999993</v>
-      </c>
-      <c r="X177" s="10">
-        <v>6.0499999999999996E-4</v>
-      </c>
-      <c r="Y177" s="9">
-        <v>1.7349235380000001</v>
-      </c>
-      <c r="Z177" s="9">
-        <v>10</v>
-      </c>
-      <c r="AA177" s="9">
-        <v>5</v>
-      </c>
-      <c r="AB177" s="9">
-        <v>5</v>
-      </c>
-      <c r="AC177" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="178" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="179" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="180" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="181" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="182" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="183" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="184" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="178" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="179" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="180" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="181" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="182" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="183" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="184" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>